<commit_message>
Running tests for CV of extra trees and pca.
</commit_message>
<xml_diff>
--- a/resources/testing_data.xlsx
+++ b/resources/testing_data.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852D291E-9295-45C8-9D82-39785399FA53}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74133E0-74B7-49BD-86BE-2507F84F3830}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="2145" windowWidth="10178" windowHeight="9720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14746" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="tree" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>Num_trees</t>
   </si>
@@ -59,6 +60,9 @@
   </si>
   <si>
     <t>end up with 25 features</t>
+  </si>
+  <si>
+    <t>Accu</t>
   </si>
 </sst>
 </file>
@@ -108,7 +112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -116,6 +120,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,8 +403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -853,4 +858,344 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80C34021-B5A8-4A8E-8025-98C033F63BB3}">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>0.6</v>
+      </c>
+      <c r="D2">
+        <v>0.95</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>0.82749999999999901</v>
+      </c>
+      <c r="G2">
+        <v>0.82627620363621901</v>
+      </c>
+      <c r="H2">
+        <v>0.83684968615489097</v>
+      </c>
+      <c r="I2">
+        <v>0.82749999999999901</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="3">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5">
+        <v>50</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.83420417431176397</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.84141171091940503</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.83499999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>50</v>
+      </c>
+      <c r="C4">
+        <v>0.6</v>
+      </c>
+      <c r="D4">
+        <v>0.95</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>0.82050000000000001</v>
+      </c>
+      <c r="G4">
+        <v>0.81965236934789998</v>
+      </c>
+      <c r="H4">
+        <v>0.82669111621986502</v>
+      </c>
+      <c r="I4">
+        <v>0.82050000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="E5" s="5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>0.82099999999999995</v>
+      </c>
+      <c r="G5">
+        <v>0.81973974747704603</v>
+      </c>
+      <c r="H5">
+        <v>0.83006417809238997</v>
+      </c>
+      <c r="I5">
+        <v>0.82099999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>50</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="E6" s="5">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0.83420417431176397</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.84141171091940503</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0.83499999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="5">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <v>100</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.83709558988570398</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.84553157280701496</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.83799999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>150</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="E8" s="5">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>0.815499999999999</v>
+      </c>
+      <c r="G8">
+        <v>0.813947617732107</v>
+      </c>
+      <c r="H8">
+        <v>0.82637552641929002</v>
+      </c>
+      <c r="I8">
+        <v>0.815499999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="5">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5">
+        <v>100</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="E9" s="5">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="G9">
+        <v>0.83604691055434499</v>
+      </c>
+      <c r="H9">
+        <v>0.84496499273709902</v>
+      </c>
+      <c r="I9">
+        <v>0.83699999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="5">
+        <v>5</v>
+      </c>
+      <c r="B10" s="5">
+        <v>100</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="E10" s="5">
+        <v>2</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.83709558988570398</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0.84553157280701496</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0.83799999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="5">
+        <v>5</v>
+      </c>
+      <c r="B11" s="5">
+        <v>100</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="E11" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" s="5">
+        <v>5</v>
+      </c>
+      <c r="B12" s="5">
+        <v>100</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="E12" s="5">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>